<commit_message>
using builtin wmma instead of rocwmma in Q @ K.T. backward optimization.
</commit_message>
<xml_diff>
--- a/brbcCalc.xlsx
+++ b/brbcCalc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26265" windowHeight="15540"/>
+    <workbookView windowWidth="24345" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="9">
   <si>
     <t>FWD</t>
   </si>
@@ -49,9 +49,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -59,27 +59,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -98,13 +77,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -113,8 +85,114 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,84 +205,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -215,187 +215,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,6 +433,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -444,6 +462,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -465,39 +498,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -514,10 +514,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -526,133 +526,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -979,10 +979,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:I14"/>
+  <dimension ref="A2:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1052,12 +1052,11 @@
         <v>64</v>
       </c>
       <c r="D5">
-        <f>A5*B5+2*(A5*C5)</f>
-        <v>24576</v>
+        <f>A5*B5+(A5*C5)</f>
+        <v>20480</v>
       </c>
       <c r="F5">
-        <f>16*14</f>
-        <v>224</v>
+        <v>256</v>
       </c>
       <c r="G5">
         <v>64</v>
@@ -1066,7 +1065,7 @@
         <v>64</v>
       </c>
       <c r="I5">
-        <f>2*(F5*G5)+G5*H5</f>
+        <f>2*(F5*G5)</f>
         <v>32768</v>
       </c>
     </row>
@@ -1078,14 +1077,14 @@
         <v>256</v>
       </c>
       <c r="C6">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D14" si="0">A6*B6+2*(A6*C6)</f>
-        <v>28672</v>
+        <f t="shared" ref="D6:D14" si="0">A6*B6+(A6*C6)</f>
+        <v>24576</v>
       </c>
       <c r="F6">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="G6">
         <v>64</v>
@@ -1094,8 +1093,8 @@
         <v>128</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I14" si="1">2*(F6*G6)+G6*H6</f>
-        <v>24576</v>
+        <f t="shared" ref="I6:I14" si="1">2*(F6*G6)</f>
+        <v>32768</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1103,7 +1102,7 @@
         <v>64</v>
       </c>
       <c r="B7">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="C7">
         <f>64*3</f>
@@ -1111,10 +1110,10 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>32768</v>
+        <v>28672</v>
       </c>
       <c r="F7">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="G7">
         <v>64</v>
@@ -1124,15 +1123,15 @@
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>28672</v>
+        <v>32768</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B8">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="C8">
         <f>64*4</f>
@@ -1140,10 +1139,10 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>30720</v>
+        <v>32768</v>
       </c>
       <c r="F8">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="G8">
         <v>64</v>
@@ -1158,10 +1157,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B9">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="C9">
         <f>64*5</f>
@@ -1175,19 +1174,19 @@
         <v>256</v>
       </c>
       <c r="G9">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="H9">
         <v>320</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>26624</v>
+        <v>32768</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B10">
         <v>128</v>
@@ -1198,20 +1197,20 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>28672</v>
+        <v>32768</v>
       </c>
       <c r="F10">
         <v>256</v>
       </c>
       <c r="G10">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="H10">
         <v>384</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>28672</v>
+        <v>32768</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1219,7 +1218,7 @@
         <v>32</v>
       </c>
       <c r="B11">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="C11">
         <f>64*7</f>
@@ -1233,19 +1232,19 @@
         <v>256</v>
       </c>
       <c r="G11">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="H11">
         <v>448</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>30720</v>
+        <v>32768</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <v>512</v>
@@ -1256,13 +1255,13 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>24576</v>
+        <v>32768</v>
       </c>
       <c r="F12">
         <v>256</v>
       </c>
       <c r="G12">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="H12">
         <v>512</v>
@@ -1274,7 +1273,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <v>256</v>
@@ -1285,28 +1284,28 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>22528</v>
+        <v>26624</v>
       </c>
       <c r="F13">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="G13">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="H13">
         <v>576</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>26624</v>
+        <v>32768</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B14">
-        <v>512</v>
+        <v>256</v>
       </c>
       <c r="C14">
         <v>640</v>
@@ -1316,16 +1315,358 @@
         <v>28672</v>
       </c>
       <c r="F14">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="G14">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="H14">
         <v>640</v>
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>64</v>
+      </c>
+      <c r="B28">
+        <v>256</v>
+      </c>
+      <c r="C28">
+        <v>64</v>
+      </c>
+      <c r="D28">
+        <f>A28*B28+2*(A28*C28)</f>
+        <v>24576</v>
+      </c>
+      <c r="F28">
+        <f>16*14</f>
+        <v>224</v>
+      </c>
+      <c r="G28">
+        <v>64</v>
+      </c>
+      <c r="H28">
+        <v>64</v>
+      </c>
+      <c r="I28">
+        <f>2*(F28*G28)+G28*H28</f>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>64</v>
+      </c>
+      <c r="B29">
+        <v>256</v>
+      </c>
+      <c r="C29">
+        <v>96</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:D37" si="2">A29*B29+2*(A29*C29)</f>
+        <v>28672</v>
+      </c>
+      <c r="F29">
+        <v>128</v>
+      </c>
+      <c r="G29">
+        <v>64</v>
+      </c>
+      <c r="H29">
+        <v>128</v>
+      </c>
+      <c r="I29">
+        <f t="shared" ref="I29:I37" si="3">2*(F29*G29)+G29*H29</f>
+        <v>24576</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>64</v>
+      </c>
+      <c r="B30">
+        <v>128</v>
+      </c>
+      <c r="C30">
+        <f>64*3</f>
+        <v>192</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>32768</v>
+      </c>
+      <c r="F30">
+        <v>128</v>
+      </c>
+      <c r="G30">
+        <v>64</v>
+      </c>
+      <c r="H30">
+        <v>192</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="3"/>
+        <v>28672</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>128</v>
+      </c>
+      <c r="C31">
+        <f>64*4</f>
+        <v>256</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>30720</v>
+      </c>
+      <c r="F31">
+        <v>128</v>
+      </c>
+      <c r="G31">
+        <v>64</v>
+      </c>
+      <c r="H31">
+        <v>256</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="3"/>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>256</v>
+      </c>
+      <c r="C32">
+        <f>64*5</f>
+        <v>320</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>28672</v>
+      </c>
+      <c r="F32">
+        <v>256</v>
+      </c>
+      <c r="G32">
+        <v>32</v>
+      </c>
+      <c r="H32">
+        <v>320</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="3"/>
+        <v>26624</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>128</v>
+      </c>
+      <c r="C33">
+        <f>64*6</f>
+        <v>384</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>28672</v>
+      </c>
+      <c r="F33">
+        <v>256</v>
+      </c>
+      <c r="G33">
+        <v>32</v>
+      </c>
+      <c r="H33">
+        <v>384</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="3"/>
+        <v>28672</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>64</v>
+      </c>
+      <c r="C34">
+        <f>64*7</f>
+        <v>448</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>30720</v>
+      </c>
+      <c r="F34">
+        <v>256</v>
+      </c>
+      <c r="G34">
+        <v>32</v>
+      </c>
+      <c r="H34">
+        <v>448</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="3"/>
+        <v>30720</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>512</v>
+      </c>
+      <c r="C35">
+        <f>64*8</f>
+        <v>512</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>24576</v>
+      </c>
+      <c r="F35">
+        <v>256</v>
+      </c>
+      <c r="G35">
+        <v>32</v>
+      </c>
+      <c r="H35">
+        <v>512</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="3"/>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <v>256</v>
+      </c>
+      <c r="C36">
+        <f>64*9</f>
+        <v>576</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>22528</v>
+      </c>
+      <c r="F36">
+        <v>128</v>
+      </c>
+      <c r="G36">
+        <v>32</v>
+      </c>
+      <c r="H36">
+        <v>576</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="3"/>
+        <v>26624</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <v>512</v>
+      </c>
+      <c r="C37">
+        <v>640</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>28672</v>
+      </c>
+      <c r="F37">
+        <v>128</v>
+      </c>
+      <c r="G37">
+        <v>32</v>
+      </c>
+      <c r="H37">
+        <v>640</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="3"/>
         <v>28672</v>
       </c>
     </row>

</xml_diff>